<commit_message>
report: shared s6 size data
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/reports/size_cores.xlsx
+++ b/docs/reports/size_cores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81302FF-47B5-4601-8B5B-31E6C6AC49FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32AE23-6A05-48CC-8992-24A0E407D1A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7366620-7C1B-460C-9134-2E5290F42A59}"/>
+    <workbookView xWindow="15375" yWindow="5085" windowWidth="14025" windowHeight="13575" xr2:uid="{F7366620-7C1B-460C-9134-2E5290F42A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Cores</t>
   </si>
   <si>
     <t>ALMs</t>
-  </si>
-  <si>
-    <t>Shared memory</t>
   </si>
   <si>
     <t>Fmax</t>
@@ -65,11 +62,41 @@
   <si>
     <t>a</t>
   </si>
+  <si>
+    <t>S_ALMs</t>
+  </si>
+  <si>
+    <t>S_ALM %</t>
+  </si>
+  <si>
+    <t>S_Regs</t>
+  </si>
+  <si>
+    <t>S_Blocks</t>
+  </si>
+  <si>
+    <t>S_Blocks %</t>
+  </si>
+  <si>
+    <t>S_Fmax</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>S_Regs %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,9 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,6 +1026,134 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-D507-49AF-A568-4696C27E7CCE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$38</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>S_ALMs</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$B$39:$B$45</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$39:$B$45</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="6">
+                        <c:v>26362</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-D507-49AF-A568-4696C27E7CCE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="8"/>
+                <c:order val="8"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$38</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>S_ALM %</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$C$39:$C$45</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$39:$C$45</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="6">
+                        <c:v>82</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{0000000A-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -2701,7 +2857,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4D87-495D-A4BF-4F310F828969}"/>
+              <c16:uniqueId val="{00000000-7996-4841-B12E-17BA18E200BA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2805,7 +2961,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4D87-495D-A4BF-4F310F828969}"/>
+              <c16:uniqueId val="{00000001-7996-4841-B12E-17BA18E200BA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2936,7 +3092,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-4D87-495D-A4BF-4F310F828969}"/>
+                    <c16:uniqueId val="{00000002-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3055,7 +3211,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-4D87-495D-A4BF-4F310F828969}"/>
+                    <c16:uniqueId val="{00000003-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3174,7 +3330,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-4D87-495D-A4BF-4F310F828969}"/>
+                    <c16:uniqueId val="{00000004-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3293,7 +3449,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000005-4D87-495D-A4BF-4F310F828969}"/>
+                    <c16:uniqueId val="{00000005-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3412,7 +3568,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000006-4D87-495D-A4BF-4F310F828969}"/>
+                    <c16:uniqueId val="{00000006-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3636,7 +3792,1916 @@
         <c:crossAx val="435275912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Regs &amp; ALMs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S_ALMs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$50:$B$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1382</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2195</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39648</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F879-4B5C-8227-C8747494FA80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S_Regs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$50:$D$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3713</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-F879-4B5C-8227-C8747494FA80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ALM Limit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$50:$I$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-F879-4B5C-8227-C8747494FA80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="435275912"/>
+        <c:axId val="435276240"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$49</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>S_ALM %</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$50:$C$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>10.24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>17.28</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>27.44</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>54</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>103</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>233</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>495</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000009-F879-4B5C-8227-C8747494FA80}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="435275912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Core Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435276240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="435276240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435275912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>ALM % </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Blocks % </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S_ALM %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3644-4C3A-B0FF-8D852D874B45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S_Blocks %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$50:$F$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3644-4C3A-B0FF-8D852D874B45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="435275912"/>
+        <c:axId val="435276240"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Regs</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$13:$D$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>886</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1322</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2201</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3844</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7328</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>14107</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>27919</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-3644-4C3A-B0FF-8D852D874B45}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>ALMs</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$13:$B$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>709</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1138</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1840</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3341</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>6522</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>12790</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>25312</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-3644-4C3A-B0FF-8D852D874B45}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Fmax</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$13:$G$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>93.86</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>82.31</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>67.959999999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>61.9</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>60.94</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>59.44</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>58.25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-3644-4C3A-B0FF-8D852D874B45}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S_Regs %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$50:$J$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6437500000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.693750000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.206250000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.631250000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.581249999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175.78749999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3644-4C3A-B0FF-8D852D874B45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="444741936"/>
+        <c:axId val="444748168"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$49</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>S_Fmax</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$F$50:$F$56</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>55</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>85</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-3644-4C3A-B0FF-8D852D874B45}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="435275912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Core Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435276240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="435276240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ALM %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435275912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="444748168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Blocks %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="444741936"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="444741936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="444748168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3840,6 +5905,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4847,6 +6992,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5442,10 +8593,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 20">
+        <xdr:cNvPr id="23" name="Chart 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5690D9-171A-4942-9E72-6DF7F41474BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFC2D34A-1D6D-4BD7-8349-B4C16F3435EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5460,6 +8611,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>604225</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>32924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name="Chart 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FE3C3E3-17EF-47BF-8F85-A4BE7E287F13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>503372</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>32924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="25" name="Chart 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABF6F69C-DF39-4559-8C94-17444970EAF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5765,19 +8992,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F796E-16F2-4844-9FB7-50E4E41A20A2}">
-  <dimension ref="A11:Z30"/>
+  <dimension ref="A12:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
@@ -5786,25 +9014,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
         <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -6012,11 +9240,387 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="Z30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
         <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>50</v>
+      </c>
+      <c r="I39">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="H40">
+        <v>50</v>
+      </c>
+      <c r="I40">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>50</v>
+      </c>
+      <c r="I41">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>50</v>
+      </c>
+      <c r="I42">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>50</v>
+      </c>
+      <c r="I43">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>32</v>
+      </c>
+      <c r="H44">
+        <v>50</v>
+      </c>
+      <c r="I44">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>64</v>
+      </c>
+      <c r="B45">
+        <v>26362</v>
+      </c>
+      <c r="C45">
+        <v>82</v>
+      </c>
+      <c r="D45">
+        <v>28768</v>
+      </c>
+      <c r="E45">
+        <v>225280</v>
+      </c>
+      <c r="F45">
+        <v>6</v>
+      </c>
+      <c r="G45">
+        <v>62.57</v>
+      </c>
+      <c r="H45">
+        <v>50</v>
+      </c>
+      <c r="I45">
+        <v>32070</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>820</v>
+      </c>
+      <c r="C50">
+        <v>10.24</v>
+      </c>
+      <c r="D50">
+        <v>804</v>
+      </c>
+      <c r="E50">
+        <v>5.5</v>
+      </c>
+      <c r="F50">
+        <v>55</v>
+      </c>
+      <c r="H50">
+        <v>50</v>
+      </c>
+      <c r="I50">
+        <v>8000</v>
+      </c>
+      <c r="J50">
+        <f>(D50/16000)*100</f>
+        <v>5.0250000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>1382</v>
+      </c>
+      <c r="C51">
+        <v>17.28</v>
+      </c>
+      <c r="D51">
+        <v>1223</v>
+      </c>
+      <c r="E51" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="F51">
+        <v>65</v>
+      </c>
+      <c r="H51">
+        <v>50</v>
+      </c>
+      <c r="I51">
+        <v>8000</v>
+      </c>
+      <c r="J51">
+        <f t="shared" ref="J51:J56" si="0">(D51/16000)*100</f>
+        <v>7.6437500000000007</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>2195</v>
+      </c>
+      <c r="C52">
+        <v>27.44</v>
+      </c>
+      <c r="D52">
+        <v>2031</v>
+      </c>
+      <c r="E52">
+        <v>8.5</v>
+      </c>
+      <c r="F52">
+        <v>85</v>
+      </c>
+      <c r="H52">
+        <v>50</v>
+      </c>
+      <c r="I52">
+        <v>8000</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>12.693750000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>8</v>
+      </c>
+      <c r="B53">
+        <v>4312</v>
+      </c>
+      <c r="C53">
+        <v>54</v>
+      </c>
+      <c r="D53">
+        <v>3713</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+      <c r="H53">
+        <v>50</v>
+      </c>
+      <c r="I53">
+        <v>8000</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>23.206250000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>16</v>
+      </c>
+      <c r="B54">
+        <v>8256</v>
+      </c>
+      <c r="C54">
+        <v>103</v>
+      </c>
+      <c r="D54">
+        <v>7301</v>
+      </c>
+      <c r="E54">
+        <v>10</v>
+      </c>
+      <c r="F54">
+        <v>100</v>
+      </c>
+      <c r="H54">
+        <v>50</v>
+      </c>
+      <c r="I54">
+        <v>8000</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>45.631250000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>32</v>
+      </c>
+      <c r="B55">
+        <v>18652</v>
+      </c>
+      <c r="C55">
+        <v>233</v>
+      </c>
+      <c r="D55">
+        <v>15933</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55">
+        <v>100</v>
+      </c>
+      <c r="H55">
+        <v>50</v>
+      </c>
+      <c r="I55">
+        <v>8000</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>99.581249999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>64</v>
+      </c>
+      <c r="B56">
+        <v>39648</v>
+      </c>
+      <c r="C56">
+        <v>495</v>
+      </c>
+      <c r="D56">
+        <v>28126</v>
+      </c>
+      <c r="E56">
+        <v>10</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>50</v>
+      </c>
+      <c r="I56">
+        <v>8000</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>175.78749999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
soc: PSEL recovery for bad PADDR values
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/reports/size_cores.xlsx
+++ b/docs/reports/size_cores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32AE23-6A05-48CC-8992-24A0E407D1A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC67EA3-A13F-4BC1-BAAB-763547D60C1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15375" yWindow="5085" windowWidth="14025" windowHeight="13575" xr2:uid="{F7366620-7C1B-460C-9134-2E5290F42A59}"/>
+    <workbookView xWindow="23970" yWindow="4260" windowWidth="14025" windowHeight="13575" xr2:uid="{F7366620-7C1B-460C-9134-2E5290F42A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Cores</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>S_Regs %</t>
+  </si>
+  <si>
+    <t>per</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
@@ -904,7 +907,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
@@ -1023,7 +1026,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
@@ -1036,7 +1039,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$38</c15:sqref>
@@ -1087,7 +1090,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
@@ -1100,7 +1103,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$38</c15:sqref>
@@ -1151,7 +1154,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-D507-49AF-A568-4696C27E7CCE}"/>
                   </c:ext>
@@ -1867,7 +1870,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-BB30-4A8D-B8D8-9309B212AFBE}"/>
                   </c:ext>
@@ -1998,7 +2001,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-BB30-4A8D-B8D8-9309B212AFBE}"/>
                   </c:ext>
@@ -2129,7 +2132,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-BB30-4A8D-B8D8-9309B212AFBE}"/>
                   </c:ext>
@@ -3209,7 +3212,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
@@ -3328,7 +3331,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
@@ -3447,7 +3450,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
@@ -3566,7 +3569,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-7996-4841-B12E-17BA18E200BA}"/>
                   </c:ext>
@@ -4966,7 +4969,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
@@ -5002,7 +5005,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$13:$B$20</c15:sqref>
@@ -5037,7 +5040,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-3644-4C3A-B0FF-8D852D874B45}"/>
                   </c:ext>
@@ -5091,7 +5094,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$13:$A$20</c15:sqref>
@@ -5127,7 +5130,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$G$13:$G$20</c15:sqref>
@@ -5162,7 +5165,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-3644-4C3A-B0FF-8D852D874B45}"/>
                   </c:ext>
@@ -8992,10 +8995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F796E-16F2-4844-9FB7-50E4E41A20A2}">
-  <dimension ref="A12:Z56"/>
+  <dimension ref="A12:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9618,6 +9621,146 @@
         <v>175.78749999999999</v>
       </c>
     </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" t="s">
+        <v>8</v>
+      </c>
+      <c r="I61" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>8000</v>
+      </c>
+      <c r="J62">
+        <f>(D62/16000)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="I63">
+        <v>8000</v>
+      </c>
+      <c r="J63">
+        <f t="shared" ref="J63:J68" si="1">(D63/16000)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="I64">
+        <v>8000</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="I65">
+        <v>8000</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="I66">
+        <v>8000</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>32</v>
+      </c>
+      <c r="B67">
+        <v>19294</v>
+      </c>
+      <c r="C67">
+        <v>241.18</v>
+      </c>
+      <c r="D67">
+        <v>14231</v>
+      </c>
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="I67">
+        <v>8000</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="1"/>
+        <v>88.943749999999994</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>64</v>
+      </c>
+      <c r="I68">
+        <v>8000</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
report: start of conclusion
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/reports/size_cores.xlsx
+++ b/docs/reports/size_cores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B517DD-5D58-4FFD-9213-8366D1980A85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0765EAEA-D640-4018-81DB-3C4E6166725B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F7366620-7C1B-460C-9134-2E5290F42A59}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>Cores</t>
   </si>

</xml_diff>